<commit_message>
Agregado de compatibilidad con archivos '.xls' y filtro de archivos permitidos en el control FileUpload
</commit_message>
<xml_diff>
--- a/PruebasPS/Planillas_Subidas/Libro1.xlsx
+++ b/PruebasPS/Planillas_Subidas/Libro1.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juanma\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja4" sheetId="1" r:id="rId3"/>
+    <sheet name="Evaluation Warning" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
   <si>
     <t>Fecha de compra (date_created)</t>
   </si>
@@ -277,13 +274,26 @@
   </si>
   <si>
     <t>https://www.mercadopago.com.ar/activities/detail/merchant_order_sale-53a900a1bcc66fe247f61289cafb003a91fb553b</t>
+  </si>
+  <si>
+    <t>Evaluation Only. Created with Aspose.Cells for .NET.Copyright 2003 - 2022 Aspose Pty Ltd.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;\ #,##0;\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;\ #,##0.00;\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,44 +303,200 @@
     </font>
     <font>
       <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color indexed="54"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -344,76 +510,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -428,175 +549,188 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -621,7 +755,6 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="double">
@@ -636,25 +769,34 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -669,7 +811,6 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -684,131 +825,243 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
       <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4" tint="0.499980002641678"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.399980008602142"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="61">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="19" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="20" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="21" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="22" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="23" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="24" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="25" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="26" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="27" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="28" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="29" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="30" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="31" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="32" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="33" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="47">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="34" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="35" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="36" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="37" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="38" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="39" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="40" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="15"/>
+    <cellStyle name="20% - Énfasis2" xfId="16"/>
+    <cellStyle name="20% - Énfasis3" xfId="17"/>
+    <cellStyle name="20% - Énfasis4" xfId="18"/>
+    <cellStyle name="20% - Énfasis5" xfId="19"/>
+    <cellStyle name="20% - Énfasis6" xfId="20"/>
+    <cellStyle name="40% - Énfasis1" xfId="21"/>
+    <cellStyle name="40% - Énfasis2" xfId="22"/>
+    <cellStyle name="40% - Énfasis3" xfId="23"/>
+    <cellStyle name="40% - Énfasis4" xfId="24"/>
+    <cellStyle name="40% - Énfasis5" xfId="25"/>
+    <cellStyle name="40% - Énfasis6" xfId="26"/>
+    <cellStyle name="60% - Énfasis1" xfId="27"/>
+    <cellStyle name="60% - Énfasis2" xfId="28"/>
+    <cellStyle name="60% - Énfasis3" xfId="29"/>
+    <cellStyle name="60% - Énfasis4" xfId="30"/>
+    <cellStyle name="60% - Énfasis5" xfId="31"/>
+    <cellStyle name="60% - Énfasis6" xfId="32"/>
+    <cellStyle name="Bueno" xfId="33"/>
+    <cellStyle name="Cálculo" xfId="34"/>
+    <cellStyle name="Celda de comprobación" xfId="35"/>
+    <cellStyle name="Celda vinculada" xfId="36"/>
+    <cellStyle name="Encabezado 1" xfId="37"/>
+    <cellStyle name="Encabezado 4" xfId="38"/>
+    <cellStyle name="Énfasis1" xfId="39"/>
+    <cellStyle name="Énfasis2" xfId="40"/>
+    <cellStyle name="Énfasis3" xfId="41"/>
+    <cellStyle name="Énfasis4" xfId="42"/>
+    <cellStyle name="Énfasis5" xfId="43"/>
+    <cellStyle name="Énfasis6" xfId="44"/>
+    <cellStyle name="Entrada" xfId="45"/>
+    <cellStyle name="Incorrecto" xfId="46"/>
+    <cellStyle name="Comma" xfId="47" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="48" builtinId="6"/>
+    <cellStyle name="Currency" xfId="49" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="50" builtinId="7"/>
+    <cellStyle name="Neutral" xfId="51"/>
+    <cellStyle name="Notas" xfId="52"/>
+    <cellStyle name="Percent" xfId="53" builtinId="5"/>
+    <cellStyle name="Salida" xfId="54"/>
+    <cellStyle name="Texto de advertencia" xfId="55"/>
+    <cellStyle name="Texto explicativo" xfId="56"/>
+    <cellStyle name="Título" xfId="57"/>
+    <cellStyle name="Título 2" xfId="58"/>
+    <cellStyle name="Título 3" xfId="59"/>
+    <cellStyle name="Total" xfId="60"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1082,16 +1335,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0cdc4173-6739-486b-bf7e-c0cececf65e7}">
   <dimension ref="A1:AQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1475,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" ht="15">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1296,7 +1549,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" ht="15">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1370,7 +1623,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" ht="15">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1444,7 +1697,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" ht="15">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1518,7 +1771,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" ht="15">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1592,7 +1845,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" ht="15">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1667,6 +1920,27 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{b51b5117-3e37-49b7-bfcb-7a97c7e3b559}">
+  <dimension ref="A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:1" ht="23.25" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregado de Listado de Registros identicos a DB
</commit_message>
<xml_diff>
--- a/PruebasPS/Planillas_Subidas/Libro1.xlsx
+++ b/PruebasPS/Planillas_Subidas/Libro1.xlsx
@@ -1,41 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xxxx\OneDrive - frgp.utn.edu.ar\Escritorio\Practicas\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9D135F-9A15-4587-A187-D004C5C740AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="2475" windowWidth="21600" windowHeight="11775" xr2:uid="{A3F6F686-98EC-4CC9-BA91-D1A210CCADE7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="mercadopago" sheetId="1" r:id="rId3"/>
+    <sheet name="Evaluation Warning" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
   <si>
     <t>Fecha de compra (date_created)</t>
   </si>
@@ -166,6 +147,15 @@
     <t>Costos de financiación (financing_fee)</t>
   </si>
   <si>
+    <t>01/06/2022 23:54:54</t>
+  </si>
+  <si>
+    <t>01/06/2022 23:54:56</t>
+  </si>
+  <si>
+    <t>19/06/2022 23:54:56</t>
+  </si>
+  <si>
     <t>ecgabrielec@hotmail.com</t>
   </si>
   <si>
@@ -202,18 +192,42 @@
     <t>https://www.mercadopago.com.ar/activities/detail/merchant_order_sale-d254dda57020eade636173c08c09303ad8157dcf</t>
   </si>
   <si>
+    <t>01/06/2022 22:59:24</t>
+  </si>
+  <si>
+    <t>01/06/2022 22:59:26</t>
+  </si>
+  <si>
+    <t>19/06/2022 22:59:26</t>
+  </si>
+  <si>
     <t>enzofconde@outlook.com.ar</t>
   </si>
   <si>
     <t>https://www.mercadopago.com.ar/activities/detail/merchant_order_sale-1f47c32237f614b3975ad991c9ed5d0a673f487b</t>
   </si>
   <si>
+    <t>01/06/2022 22:19:58</t>
+  </si>
+  <si>
+    <t>01/06/2022 22:20:02</t>
+  </si>
+  <si>
+    <t>19/06/2022 22:20:02</t>
+  </si>
+  <si>
     <t>matias_morales_1996@hotmail.com</t>
   </si>
   <si>
     <t>https://www.mercadopago.com.ar/activities/detail/merchant_order_sale-ca5fd47ead214551478dc27949df85c2cbc87fcb</t>
   </si>
   <si>
+    <t>01/06/2022 22:06:53</t>
+  </si>
+  <si>
+    <t>19/06/2022 22:06:53</t>
+  </si>
+  <si>
     <t>santii.hidalgo@gmail.com</t>
   </si>
   <si>
@@ -232,23 +246,43 @@
     <t>https://www.mercadopago.com.ar/activities/detail/merchant_order_sale-2a2a5557a8f1d959fe9d3edb7dfd6dad5644f87b</t>
   </si>
   <si>
+    <t>01/06/2022 21:54:55</t>
+  </si>
+  <si>
+    <t>01/06/2022 21:54:57</t>
+  </si>
+  <si>
+    <t>19/06/2022 21:54:57</t>
+  </si>
+  <si>
     <t>sebastian.ezequiel94@gmail.com</t>
   </si>
   <si>
     <t>https://www.mercadopago.com.ar/activities/detail/merchant_order_sale-5a7f8b1dc23ce1aec1ecd5bb1799257d6544bfae</t>
   </si>
   <si>
-    <t>federicoescobarf.e@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.mercadopago.com.ar/activities/detail/merchant_order_sale-53a900a1bcc66fe247f61289cafb003a91fb553b</t>
+    <t>Evaluation Only. Created with Aspose.Cells for .NET.Copyright 2003 - 2022 Aspose Pty Ltd.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="12">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;\ #,##0;\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;\ #,##0.00;\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;Sí&quot;;&quot;Sí&quot;;&quot;No&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;Verdadero&quot;;&quot;Verdadero&quot;;&quot;Falso&quot;"/>
+    <numFmt numFmtId="166" formatCode="&quot;Activado&quot;;&quot;Activado&quot;;&quot;Desactivado&quot;"/>
+    <numFmt numFmtId="167" formatCode="[$€-2]\ #,##0.00_);[Red]\([$€-2]\ #,##0.00\)"/>
+  </numFmts>
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,16 +290,458 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color indexed="54"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="22"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFDCDDDE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799979984760284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599990010261536"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399980008602142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -273,19 +749,332 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4" tint="0.499980002641678"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.399980008602142"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="61">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="47">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Énfasis1" xfId="15"/>
+    <cellStyle name="20% - Énfasis2" xfId="16"/>
+    <cellStyle name="20% - Énfasis3" xfId="17"/>
+    <cellStyle name="20% - Énfasis4" xfId="18"/>
+    <cellStyle name="20% - Énfasis5" xfId="19"/>
+    <cellStyle name="20% - Énfasis6" xfId="20"/>
+    <cellStyle name="40% - Énfasis1" xfId="21"/>
+    <cellStyle name="40% - Énfasis2" xfId="22"/>
+    <cellStyle name="40% - Énfasis3" xfId="23"/>
+    <cellStyle name="40% - Énfasis4" xfId="24"/>
+    <cellStyle name="40% - Énfasis5" xfId="25"/>
+    <cellStyle name="40% - Énfasis6" xfId="26"/>
+    <cellStyle name="60% - Énfasis1" xfId="27"/>
+    <cellStyle name="60% - Énfasis2" xfId="28"/>
+    <cellStyle name="60% - Énfasis3" xfId="29"/>
+    <cellStyle name="60% - Énfasis4" xfId="30"/>
+    <cellStyle name="60% - Énfasis5" xfId="31"/>
+    <cellStyle name="60% - Énfasis6" xfId="32"/>
+    <cellStyle name="Bueno" xfId="33"/>
+    <cellStyle name="Cálculo" xfId="34"/>
+    <cellStyle name="Celda de comprobación" xfId="35"/>
+    <cellStyle name="Celda vinculada" xfId="36"/>
+    <cellStyle name="Encabezado 1" xfId="37"/>
+    <cellStyle name="Encabezado 4" xfId="38"/>
+    <cellStyle name="Énfasis1" xfId="39"/>
+    <cellStyle name="Énfasis2" xfId="40"/>
+    <cellStyle name="Énfasis3" xfId="41"/>
+    <cellStyle name="Énfasis4" xfId="42"/>
+    <cellStyle name="Énfasis5" xfId="43"/>
+    <cellStyle name="Énfasis6" xfId="44"/>
+    <cellStyle name="Entrada" xfId="45"/>
+    <cellStyle name="Incorrecto" xfId="46"/>
+    <cellStyle name="Comma" xfId="47" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="48" builtinId="6"/>
+    <cellStyle name="Currency" xfId="49" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="50" builtinId="7"/>
+    <cellStyle name="Neutral" xfId="51"/>
+    <cellStyle name="Notas" xfId="52"/>
+    <cellStyle name="Percent" xfId="53" builtinId="5"/>
+    <cellStyle name="Salida" xfId="54"/>
+    <cellStyle name="Texto de advertencia" xfId="55"/>
+    <cellStyle name="Texto explicativo" xfId="56"/>
+    <cellStyle name="Título" xfId="57"/>
+    <cellStyle name="Título 2" xfId="58"/>
+    <cellStyle name="Título 3" xfId="59"/>
+    <cellStyle name="Total" xfId="60"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -314,7 +1103,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -326,7 +1115,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -373,23 +1162,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -425,23 +1197,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -593,19 +1348,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9C0AC3-F1AA-41A2-A7E5-465B34A77B01}">
-  <dimension ref="A1:AQ7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6c8a1b02-78cc-4d72-8aa5-7628ad5c7639}">
+  <dimension ref="A1:AQ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="11" max="11" width="47.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -636,7 +1388,7 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" t="s">
@@ -736,451 +1488,401 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>44713.995833333334</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44713.995833333334</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44731.995833333334</v>
+    <row r="2" spans="1:43" ht="15">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I2">
         <v>6234808</v>
       </c>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K2">
-        <v>47907</v>
+        <v>47528</v>
       </c>
       <c r="M2">
         <v>22824396111</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="R2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="S2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="T2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="U2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="V2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="W2">
         <v>1</v>
       </c>
       <c r="X2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Y2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AC2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AE2">
         <v>4878371278</v>
       </c>
       <c r="AH2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AQ2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>44713.957638888889</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44713.957638888889</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44731.957638888889</v>
+    <row r="3" spans="1:43" ht="15">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="I3">
         <v>6234672</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K3">
-        <v>47908</v>
+        <v>47776</v>
       </c>
       <c r="M3">
         <v>22823481682</v>
       </c>
       <c r="N3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="R3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="S3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="T3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="U3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="V3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="W3">
         <v>1</v>
       </c>
       <c r="X3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Y3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AC3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AE3">
         <v>4878139306</v>
       </c>
       <c r="AH3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="AQ3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>44713.929861111108</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44713.930555555555</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44731.930555555555</v>
+    <row r="4" spans="1:43" ht="15">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="I4">
         <v>6234134</v>
       </c>
       <c r="J4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K4">
-        <v>47917</v>
+        <v>47777</v>
       </c>
       <c r="M4">
         <v>22822691994</v>
       </c>
       <c r="N4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="R4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="S4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="T4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="U4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="V4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="W4">
         <v>1</v>
       </c>
       <c r="X4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Y4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AC4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AE4">
         <v>4877922515</v>
       </c>
       <c r="AH4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="AQ4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>44713.92083333333</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44713.92083333333</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44731.92083333333</v>
+    <row r="5" spans="1:43" ht="15">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="I5">
         <v>6208632</v>
       </c>
       <c r="J5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K5">
-        <v>47916</v>
+        <v>47778</v>
       </c>
       <c r="M5">
         <v>22822390789</v>
       </c>
       <c r="N5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="R5" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="S5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="T5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="U5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="V5" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="W5">
         <v>1</v>
       </c>
       <c r="X5" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="Y5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AC5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AE5">
         <v>4877840387</v>
       </c>
       <c r="AH5" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="AQ5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>44713.912499999999</v>
-      </c>
-      <c r="B6" s="1">
-        <v>44713.912499999999</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44731.912499999999</v>
+    <row r="6" spans="1:43" ht="15">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="I6">
         <v>6234446</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K6">
-        <v>47918</v>
+        <v>47790</v>
       </c>
       <c r="M6">
         <v>22822092929</v>
       </c>
       <c r="N6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="R6" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="S6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="T6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="U6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="V6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="W6">
         <v>1</v>
       </c>
       <c r="X6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Y6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AC6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AE6">
         <v>4877761870</v>
       </c>
       <c r="AH6" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="AQ6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>44713.89166666667</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44713.89166666667</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44731.89166666667</v>
-      </c>
-      <c r="F7" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7">
-        <v>6234570</v>
-      </c>
-      <c r="J7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7">
-        <v>47919</v>
-      </c>
-      <c r="M7">
-        <v>22821306240</v>
-      </c>
-      <c r="N7" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" t="s">
-        <v>46</v>
-      </c>
-      <c r="P7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R7" t="s">
-        <v>49</v>
-      </c>
-      <c r="S7" t="s">
-        <v>50</v>
-      </c>
-      <c r="T7" t="s">
-        <v>50</v>
-      </c>
-      <c r="U7" t="s">
-        <v>50</v>
-      </c>
-      <c r="V7" t="s">
-        <v>51</v>
-      </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
-      <c r="X7" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE7">
-        <v>4877545130</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>50</v>
-      </c>
+    <row r="11" spans="4:4" ht="15.75">
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
+  <sheetProtection/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup horizontalDpi="300" verticalDpi="300" orientation="portrait" paperSize="9" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8f09c853-7e1e-48c2-b6d0-317ad78f242e}">
+  <dimension ref="A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:1" ht="23.25" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Armado reporte de resultado final
</commit_message>
<xml_diff>
--- a/PruebasPS/Planillas_Subidas/Libro1.xlsx
+++ b/PruebasPS/Planillas_Subidas/Libro1.xlsx
@@ -1348,11 +1348,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6c8a1b02-78cc-4d72-8aa5-7628ad5c7639}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{f385981e-7b2c-4ad9-88d8-71d36bc66f3f}">
   <dimension ref="A1:AQ11"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="topLeft" activeCell="K2" sqref="K2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1508,7 +1508,7 @@
         <v>47</v>
       </c>
       <c r="K2">
-        <v>47528</v>
+        <v>47565</v>
       </c>
       <c r="M2">
         <v>22824396111</v>
@@ -1582,7 +1582,7 @@
         <v>47</v>
       </c>
       <c r="K3">
-        <v>47776</v>
+        <v>47594</v>
       </c>
       <c r="M3">
         <v>22823481682</v>
@@ -1656,7 +1656,7 @@
         <v>47</v>
       </c>
       <c r="K4">
-        <v>47777</v>
+        <v>47629</v>
       </c>
       <c r="M4">
         <v>22822691994</v>
@@ -1730,7 +1730,7 @@
         <v>47</v>
       </c>
       <c r="K5">
-        <v>47778</v>
+        <v>47651</v>
       </c>
       <c r="M5">
         <v>22822390789</v>
@@ -1804,7 +1804,7 @@
         <v>47</v>
       </c>
       <c r="K6">
-        <v>47790</v>
+        <v>47659</v>
       </c>
       <c r="M6">
         <v>22822092929</v>
@@ -1869,7 +1869,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8f09c853-7e1e-48c2-b6d0-317ad78f242e}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1612ae56-2d75-466e-80a7-aeffad03a1db}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>

</xml_diff>

<commit_message>
Estilo botón 'Procesar Archivo'
</commit_message>
<xml_diff>
--- a/PruebasPS/Planillas_Subidas/Libro1.xlsx
+++ b/PruebasPS/Planillas_Subidas/Libro1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="1"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="24000" windowHeight="9600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mercadopago" sheetId="1" r:id="rId3"/>
@@ -1339,20 +1339,15 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{f385981e-7b2c-4ad9-88d8-71d36bc66f3f}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{a88ed688-3e28-4e2b-a14d-27ded70b7b17}">
   <dimension ref="A1:AQ11"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="K2" sqref="K2:K6"/>
+      <selection pane="topLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1508,7 +1503,7 @@
         <v>47</v>
       </c>
       <c r="K2">
-        <v>47565</v>
+        <v>47662</v>
       </c>
       <c r="M2">
         <v>22824396111</v>
@@ -1582,7 +1577,7 @@
         <v>47</v>
       </c>
       <c r="K3">
-        <v>47594</v>
+        <v>47673</v>
       </c>
       <c r="M3">
         <v>22823481682</v>
@@ -1656,7 +1651,7 @@
         <v>47</v>
       </c>
       <c r="K4">
-        <v>47629</v>
+        <v>47674</v>
       </c>
       <c r="M4">
         <v>22822691994</v>
@@ -1730,7 +1725,7 @@
         <v>47</v>
       </c>
       <c r="K5">
-        <v>47651</v>
+        <v>47684</v>
       </c>
       <c r="M5">
         <v>22822390789</v>
@@ -1804,7 +1799,7 @@
         <v>47</v>
       </c>
       <c r="K6">
-        <v>47659</v>
+        <v>47687</v>
       </c>
       <c r="M6">
         <v>22822092929</v>
@@ -1869,7 +1864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1612ae56-2d75-466e-80a7-aeffad03a1db}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ebf9a294-5229-4e0c-9491-f71125cc9255}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>

</xml_diff>